<commit_message>
-Controllers and Views generated
</commit_message>
<xml_diff>
--- a/web-app/files/counselor.xlsx
+++ b/web-app/files/counselor.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="600">
   <si>
     <t>Mtgs Attended</t>
   </si>
@@ -269,6 +269,9 @@
     <t>(562) 240-7479</t>
   </si>
   <si>
+    <t>K1</t>
+  </si>
+  <si>
     <t>Maritza Escobar</t>
   </si>
   <si>
@@ -471,6 +474,9 @@
   </si>
   <si>
     <t>(562)544-7165</t>
+  </si>
+  <si>
+    <t>TK</t>
   </si>
   <si>
     <t>Lucina Gutierrez</t>
@@ -2028,8 +2034,8 @@
   </sheetPr>
   <dimension ref="A1:AK110"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A88" activeCellId="0" sqref="A88"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Z28" activeCellId="0" sqref="Z28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2374,14 +2380,17 @@
       <c r="Y4" s="4" t="s">
         <v>83</v>
       </c>
+      <c r="Z4" s="0" t="s">
+        <v>84</v>
+      </c>
       <c r="AA4" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AB4" s="4" t="s">
         <v>54</v>
       </c>
       <c r="AC4" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AF4" s="5" t="n">
         <v>18</v>
@@ -2392,31 +2401,31 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>39</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K5" s="5" t="n">
         <v>25</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>61</v>
@@ -2431,37 +2440,37 @@
         <v>46</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="V5" s="4" t="s">
         <v>49</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="X5" s="4" t="s">
         <v>51</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="Z5" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AA5" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AB5" s="4" t="s">
         <v>54</v>
       </c>
       <c r="AC5" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AF5" s="5" t="n">
         <v>25</v>
@@ -2479,25 +2488,25 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>41</v>
@@ -2506,7 +2515,7 @@
         <v>24</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>61</v>
@@ -2521,22 +2530,22 @@
         <v>46</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="V6" s="4" t="s">
         <v>49</v>
       </c>
       <c r="X6" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="Z6" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AB6" s="4" t="s">
         <v>54</v>
@@ -2556,76 +2565,76 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K7" s="5" t="n">
         <v>17</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N7" s="4" t="s">
         <v>62</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="P7" s="4" t="s">
         <v>76</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="V7" s="4" t="s">
         <v>59</v>
       </c>
       <c r="W7" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="X7" s="4" t="s">
         <v>82</v>
       </c>
       <c r="Z7" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AA7" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AB7" s="4" t="s">
         <v>54</v>
       </c>
       <c r="AC7" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AF7" s="5" t="n">
         <v>17</v>
@@ -2636,70 +2645,70 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>62</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K8" s="5" t="n">
         <v>23</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N8" s="4" t="s">
         <v>62</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="P8" s="4" t="s">
         <v>76</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="V8" s="4" t="s">
         <v>49</v>
       </c>
       <c r="W8" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="X8" s="4" t="s">
         <v>64</v>
       </c>
       <c r="Y8" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="Z8" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AA8" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AB8" s="4" t="s">
         <v>54</v>
@@ -2719,31 +2728,31 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>58</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K9" s="5" t="n">
         <v>23</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M9" s="4" t="s">
         <v>61</v>
@@ -2758,37 +2767,37 @@
         <v>46</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="V9" s="4" t="s">
         <v>49</v>
       </c>
       <c r="W9" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="X9" s="4" t="s">
         <v>51</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="Z9" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="AA9" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AB9" s="4" t="s">
         <v>54</v>
       </c>
       <c r="AC9" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AF9" s="5" t="n">
         <v>23</v>
@@ -2805,34 +2814,34 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K10" s="5" t="n">
         <v>19</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>61</v>
@@ -2847,34 +2856,37 @@
         <v>46</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="V10" s="4" t="s">
         <v>49</v>
       </c>
       <c r="W10" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="X10" s="4" t="s">
         <v>51</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
+      </c>
+      <c r="Z10" s="0" t="s">
+        <v>153</v>
       </c>
       <c r="AA10" s="4" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AB10" s="4" t="s">
         <v>54</v>
       </c>
       <c r="AC10" s="4" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="AF10" s="5" t="n">
         <v>19</v>
@@ -2885,34 +2897,34 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="4" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>39</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="K11" s="5" t="n">
         <v>16</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="M11" s="4" t="s">
         <v>74</v>
@@ -2921,43 +2933,43 @@
         <v>62</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="P11" s="4" t="s">
         <v>76</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="S11" s="4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="V11" s="4" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="W11" s="4" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="X11" s="4" t="s">
         <v>51</v>
       </c>
       <c r="Y11" s="4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="Z11" s="4" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="AA11" s="4" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="AB11" s="4" t="s">
         <v>54</v>
       </c>
       <c r="AC11" s="4" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="AF11" s="5" t="n">
         <v>16</v>
@@ -2968,37 +2980,37 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="4" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>69</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K12" s="5" t="n">
         <v>17</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>61</v>
@@ -3013,34 +3025,37 @@
         <v>46</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="S12" s="4" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="V12" s="4" t="s">
         <v>59</v>
       </c>
       <c r="W12" s="4" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="X12" s="4" t="s">
         <v>51</v>
       </c>
       <c r="Y12" s="4" t="s">
-        <v>177</v>
+        <v>179</v>
+      </c>
+      <c r="Z12" s="0" t="s">
+        <v>84</v>
       </c>
       <c r="AA12" s="4" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AB12" s="4" t="s">
         <v>54</v>
       </c>
       <c r="AC12" s="4" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="AF12" s="5" t="n">
         <v>17</v>
@@ -3051,19 +3066,19 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="4" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>58</v>
@@ -3072,49 +3087,52 @@
         <v>80</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="K13" s="5" t="n">
         <v>16</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>62</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="P13" s="4" t="s">
         <v>76</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="S13" s="4" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="U13" s="4" t="s">
         <v>36</v>
       </c>
       <c r="V13" s="4" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="X13" s="4" t="s">
         <v>82</v>
       </c>
+      <c r="Z13" s="0" t="s">
+        <v>84</v>
+      </c>
       <c r="AA13" s="4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AB13" s="4" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="AC13" s="4" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="AF13" s="5" t="n">
         <v>16</v>
@@ -3122,34 +3140,34 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="4" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>69</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="K14" s="5" t="n">
         <v>16</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="M14" s="4" t="s">
         <v>61</v>
@@ -3164,13 +3182,13 @@
         <v>46</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="S14" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="U14" s="4" t="s">
         <v>36</v>
@@ -3179,22 +3197,25 @@
         <v>59</v>
       </c>
       <c r="W14" s="4" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="X14" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="Y14" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
+      </c>
+      <c r="Z14" s="0" t="s">
+        <v>84</v>
       </c>
       <c r="AA14" s="4" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="AB14" s="4" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="AC14" s="4" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="AF14" s="5" t="n">
         <v>16</v>
@@ -3202,70 +3223,73 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="4" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>40</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="K15" s="5" t="n">
         <v>14</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>62</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="P15" s="4" t="s">
         <v>76</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="S15" s="4" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="U15" s="4" t="s">
         <v>36</v>
       </c>
       <c r="V15" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="W15" s="4" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="X15" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
+      </c>
+      <c r="Z15" s="0" t="s">
+        <v>84</v>
       </c>
       <c r="AA15" s="4" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="AB15" s="4" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="AC15" s="4" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="AF15" s="5" t="n">
         <v>14</v>
@@ -3274,76 +3298,79 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="4" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>69</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="K16" s="5" t="n">
         <v>14</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>62</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="P16" s="4" t="s">
         <v>76</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="U16" s="4" t="s">
         <v>36</v>
       </c>
       <c r="V16" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="W16" s="4" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="X16" s="4" t="s">
         <v>82</v>
       </c>
       <c r="Y16" s="4" t="s">
-        <v>222</v>
+        <v>224</v>
+      </c>
+      <c r="Z16" s="0" t="s">
+        <v>84</v>
       </c>
       <c r="AA16" s="4" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="AB16" s="4" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="AC16" s="4" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="AF16" s="5" t="n">
         <v>14</v>
@@ -3352,73 +3379,76 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="4" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K17" s="5" t="n">
         <v>17</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>62</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="P17" s="4" t="s">
         <v>76</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="S17" s="4" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="U17" s="4" t="s">
         <v>36</v>
       </c>
       <c r="V17" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="W17" s="4" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="X17" s="4" t="s">
         <v>82</v>
       </c>
       <c r="Y17" s="4" t="s">
-        <v>232</v>
+        <v>234</v>
+      </c>
+      <c r="Z17" s="0" t="s">
+        <v>84</v>
       </c>
       <c r="AA17" s="4" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AB17" s="4" t="s">
         <v>54</v>
       </c>
       <c r="AC17" s="4" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="AF17" s="5" t="n">
         <v>17</v>
@@ -3426,31 +3456,31 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="4" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="K18" s="5" t="n">
         <v>15</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>61</v>
@@ -3459,25 +3489,28 @@
         <v>62</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="P18" s="4" t="s">
         <v>76</v>
       </c>
       <c r="R18" s="4" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="S18" s="4" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="U18" s="4" t="s">
         <v>36</v>
       </c>
       <c r="V18" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
+      </c>
+      <c r="Z18" s="0" t="s">
+        <v>153</v>
       </c>
       <c r="AB18" s="4" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="AF18" s="5" t="n">
         <v>15</v>
@@ -3485,34 +3518,34 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="4" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="K19" s="5" t="n">
         <v>16</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>61</v>
@@ -3527,37 +3560,40 @@
         <v>76</v>
       </c>
       <c r="Q19" s="4" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="S19" s="4" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="U19" s="4" t="s">
         <v>36</v>
       </c>
       <c r="V19" s="4" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="W19" s="4" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="X19" s="4" t="s">
         <v>51</v>
       </c>
       <c r="Y19" s="4" t="s">
-        <v>250</v>
+        <v>252</v>
+      </c>
+      <c r="Z19" s="0" t="s">
+        <v>153</v>
       </c>
       <c r="AA19" s="4" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AB19" s="4" t="s">
         <v>54</v>
       </c>
       <c r="AC19" s="4" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AF19" s="5" t="n">
         <v>16</v>
@@ -3565,167 +3601,176 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="4" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>70</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K20" s="5" t="n">
         <v>17</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="N20" s="4" t="s">
         <v>62</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="P20" s="4" t="s">
         <v>76</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="R20" s="4" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="S20" s="4" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="U20" s="4" t="s">
         <v>36</v>
       </c>
       <c r="V20" s="4" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="X20" s="4" t="s">
         <v>51</v>
       </c>
+      <c r="Z20" s="0" t="s">
+        <v>153</v>
+      </c>
       <c r="AA20" s="4" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="AB20" s="4" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="AC20" s="4" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="AF20" s="5" t="n">
         <v>17</v>
       </c>
       <c r="AI20" s="4" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="4" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
+      </c>
+      <c r="Z21" s="0" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="4" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="K22" s="5" t="n">
         <v>14</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N22" s="4" t="s">
         <v>62</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="P22" s="4" t="s">
         <v>46</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="S22" s="4" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="U22" s="4" t="s">
         <v>36</v>
       </c>
       <c r="V22" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="W22" s="4" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="X22" s="4" t="s">
         <v>51</v>
       </c>
       <c r="Y22" s="4" t="s">
-        <v>271</v>
+        <v>273</v>
+      </c>
+      <c r="Z22" s="0" t="s">
+        <v>153</v>
       </c>
       <c r="AA22" s="4" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="AB22" s="4" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="AC22" s="4" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="AF22" s="5" t="n">
         <v>14</v>
@@ -3733,76 +3778,79 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="4" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>69</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="K23" s="5" t="n">
         <v>16</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N23" s="4" t="s">
         <v>62</v>
       </c>
       <c r="O23" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="P23" s="4" t="s">
         <v>76</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="S23" s="4" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="U23" s="4" t="s">
         <v>36</v>
       </c>
       <c r="V23" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="W23" s="4" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="X23" s="4" t="s">
         <v>82</v>
       </c>
       <c r="Y23" s="4" t="s">
-        <v>283</v>
+        <v>285</v>
+      </c>
+      <c r="Z23" s="0" t="s">
+        <v>153</v>
       </c>
       <c r="AA23" s="4" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="AB23" s="4" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="AC23" s="4" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="AF23" s="5" t="n">
         <v>16</v>
@@ -3810,52 +3858,52 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="4" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="K24" s="5" t="n">
         <v>16</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N24" s="4" t="s">
         <v>62</v>
       </c>
       <c r="O24" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="P24" s="4" t="s">
         <v>76</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="S24" s="4" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="U24" s="4" t="s">
         <v>36</v>
@@ -3864,22 +3912,25 @@
         <v>59</v>
       </c>
       <c r="W24" s="4" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="X24" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="Y24" s="4" t="s">
-        <v>293</v>
+        <v>295</v>
+      </c>
+      <c r="Z24" s="0" t="s">
+        <v>153</v>
       </c>
       <c r="AA24" s="4" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="AB24" s="4" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="AC24" s="4" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="AF24" s="5" t="n">
         <v>16</v>
@@ -3887,49 +3938,49 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="4" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>69</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K25" s="5" t="n">
         <v>17</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N25" s="4" t="s">
         <v>62</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="Q25" s="4" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="S25" s="4" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="U25" s="4" t="s">
         <v>36</v>
@@ -3938,22 +3989,25 @@
         <v>80</v>
       </c>
       <c r="W25" s="4" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="X25" s="4" t="s">
         <v>51</v>
       </c>
       <c r="Y25" s="4" t="s">
-        <v>304</v>
+        <v>306</v>
+      </c>
+      <c r="Z25" s="0" t="s">
+        <v>153</v>
       </c>
       <c r="AA25" s="4" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="AB25" s="4" t="s">
         <v>54</v>
       </c>
       <c r="AC25" s="4" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="AF25" s="5" t="n">
         <v>17</v>
@@ -3961,37 +4015,37 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="4" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="K26" s="5" t="n">
         <v>16</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="N26" s="4" t="s">
         <v>62</v>
@@ -4003,34 +4057,37 @@
         <v>76</v>
       </c>
       <c r="Q26" s="4" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="R26" s="4" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="U26" s="4" t="s">
         <v>36</v>
       </c>
       <c r="V26" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="W26" s="4" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="X26" s="4" t="s">
         <v>51</v>
       </c>
       <c r="Y26" s="4" t="s">
-        <v>315</v>
+        <v>317</v>
+      </c>
+      <c r="Z26" s="0" t="s">
+        <v>153</v>
       </c>
       <c r="AA26" s="4" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="AB26" s="4" t="s">
         <v>54</v>
       </c>
       <c r="AC26" s="4" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="AF26" s="5" t="n">
         <v>16</v>
@@ -4038,76 +4095,79 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="4" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K27" s="5" t="n">
         <v>17</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N27" s="4" t="s">
         <v>62</v>
       </c>
       <c r="O27" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="P27" s="4" t="s">
         <v>76</v>
       </c>
       <c r="Q27" s="4" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="R27" s="4" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="S27" s="4" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="U27" s="4" t="s">
         <v>36</v>
       </c>
       <c r="V27" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="W27" s="4" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="X27" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="Y27" s="4" t="s">
-        <v>326</v>
+        <v>328</v>
+      </c>
+      <c r="Z27" s="0" t="s">
+        <v>153</v>
       </c>
       <c r="AA27" s="4" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="AB27" s="4" t="s">
         <v>54</v>
       </c>
       <c r="AC27" s="4" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="AF27" s="5" t="n">
         <v>17</v>
@@ -4115,49 +4175,49 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="4" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>71</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="K28" s="5" t="n">
         <v>15</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>62</v>
       </c>
       <c r="O28" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="P28" s="4" t="s">
         <v>46</v>
       </c>
       <c r="Q28" s="4" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="S28" s="4" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="U28" s="4" t="s">
         <v>36</v>
@@ -4166,16 +4226,16 @@
         <v>59</v>
       </c>
       <c r="X28" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="AA28" s="4" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="AB28" s="4" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="AC28" s="4" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="AF28" s="5" t="n">
         <v>15</v>
@@ -4183,79 +4243,79 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="4" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>69</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>40</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K29" s="5" t="n">
         <v>17</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>62</v>
       </c>
       <c r="O29" s="4" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="P29" s="4" t="s">
         <v>76</v>
       </c>
       <c r="Q29" s="4" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="R29" s="4" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="S29" s="4" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="U29" s="4" t="s">
         <v>36</v>
       </c>
       <c r="V29" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="W29" s="4" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="X29" s="4" t="s">
         <v>82</v>
       </c>
       <c r="Y29" s="4" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="AA29" s="4" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="AB29" s="4" t="s">
         <v>54</v>
       </c>
       <c r="AC29" s="4" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="AF29" s="5" t="n">
         <v>17</v>
@@ -4263,16 +4323,16 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="4" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>69</v>
@@ -4281,37 +4341,37 @@
         <v>70</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="K30" s="5" t="n">
         <v>16</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="N30" s="4" t="s">
         <v>62</v>
       </c>
       <c r="O30" s="4" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="P30" s="4" t="s">
         <v>76</v>
       </c>
       <c r="Q30" s="4" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="R30" s="4" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="S30" s="4" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="U30" s="4" t="s">
         <v>36</v>
@@ -4320,22 +4380,22 @@
         <v>59</v>
       </c>
       <c r="W30" s="4" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="X30" s="4" t="s">
         <v>51</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="AA30" s="4" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="AB30" s="4" t="s">
         <v>54</v>
       </c>
       <c r="AC30" s="4" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="AF30" s="5" t="n">
         <v>16</v>
@@ -4343,79 +4403,79 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="4" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>69</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K31" s="5" t="n">
         <v>17</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="N31" s="4" t="s">
         <v>62</v>
       </c>
       <c r="O31" s="4" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="P31" s="4" t="s">
         <v>76</v>
       </c>
       <c r="Q31" s="4" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="R31" s="4" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="S31" s="4" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="U31" s="4" t="s">
         <v>36</v>
       </c>
       <c r="V31" s="4" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="W31" s="4" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="X31" s="4" t="s">
         <v>82</v>
       </c>
       <c r="Y31" s="4" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="AA31" s="4" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="AB31" s="4" t="s">
         <v>54</v>
       </c>
       <c r="AC31" s="4" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="AF31" s="5" t="n">
         <v>17</v>
@@ -4423,31 +4483,31 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="4" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="K32" s="5" t="n">
         <v>16</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="M32" s="4" t="s">
         <v>61</v>
@@ -4462,34 +4522,34 @@
         <v>76</v>
       </c>
       <c r="Q32" s="4" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="S32" s="4" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="U32" s="4" t="s">
         <v>36</v>
       </c>
       <c r="V32" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="W32" s="4" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="X32" s="4" t="s">
         <v>82</v>
       </c>
       <c r="Y32" s="4" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="AA32" s="4" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="AB32" s="4" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="AC32" s="4" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="AF32" s="5" t="n">
         <v>16</v>
@@ -4498,34 +4558,34 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="4" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>69</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="K33" s="5" t="n">
         <v>14</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="M33" s="4" t="s">
         <v>61</v>
@@ -4540,37 +4600,37 @@
         <v>76</v>
       </c>
       <c r="Q33" s="4" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="R33" s="4" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="S33" s="4" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="U33" s="4" t="s">
         <v>36</v>
       </c>
       <c r="V33" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="W33" s="4" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="X33" s="4" t="s">
         <v>82</v>
       </c>
       <c r="Y33" s="4" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="AA33" s="4" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="AB33" s="4" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="AC33" s="4" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="AF33" s="5" t="n">
         <v>14</v>
@@ -4578,31 +4638,31 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="4" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="K34" s="5" t="n">
         <v>16</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="M34" s="4" t="s">
         <v>74</v>
@@ -4611,40 +4671,40 @@
         <v>62</v>
       </c>
       <c r="O34" s="4" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="P34" s="4" t="s">
         <v>76</v>
       </c>
       <c r="Q34" s="4" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="S34" s="4" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="U34" s="4" t="s">
         <v>36</v>
       </c>
       <c r="V34" s="4" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="W34" s="4" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="X34" s="4" t="s">
         <v>82</v>
       </c>
       <c r="Y34" s="4" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="AA34" s="4" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="AB34" s="4" t="s">
         <v>54</v>
       </c>
       <c r="AC34" s="4" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="AF34" s="5" t="n">
         <v>16</v>
@@ -4652,31 +4712,31 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="4" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="K35" s="5" t="n">
         <v>21</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="M35" s="4" t="s">
         <v>61</v>
@@ -4691,37 +4751,37 @@
         <v>46</v>
       </c>
       <c r="Q35" s="4" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="R35" s="4" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="S35" s="4" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="U35" s="4" t="s">
         <v>36</v>
       </c>
       <c r="V35" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="W35" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="X35" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y35" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="X35" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="Y35" s="4" t="s">
-        <v>408</v>
-      </c>
       <c r="AA35" s="4" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="AB35" s="4" t="s">
         <v>54</v>
       </c>
       <c r="AC35" s="4" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="AF35" s="5" t="n">
         <v>21</v>
@@ -4729,51 +4789,51 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="4" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="X36" s="4" t="s">
         <v>82</v>
       </c>
       <c r="AB36" s="4" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="4" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="I37" s="4" t="s">
         <v>71</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K37" s="5" t="n">
         <v>17</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="AF37" s="5" t="n">
         <v>17</v>
@@ -4781,66 +4841,66 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="4" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="4" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="4" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="4" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="4" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>61</v>
@@ -4848,13 +4908,13 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="4" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>61</v>
@@ -4862,13 +4922,13 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="4" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>61</v>
@@ -4885,87 +4945,87 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="4" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="4" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="4" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="4" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD48" s="4" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="4" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>69</v>
@@ -4973,16 +5033,16 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="4" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>69</v>
@@ -4990,16 +5050,16 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="4" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>69</v>
@@ -5007,16 +5067,16 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="4" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>69</v>
@@ -5024,65 +5084,65 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="4" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD54" s="4" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="AI54" s="4" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="4" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="4" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="K56" s="5" t="n">
         <v>15</v>
@@ -5099,33 +5159,33 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="4" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="4" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>69</v>
@@ -5133,33 +5193,33 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="4" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="F59" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="4" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>69</v>
@@ -5167,73 +5227,73 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="4" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="4" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="4" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="4" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>69</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="I64" s="4" t="s">
         <v>59</v>
@@ -5245,46 +5305,46 @@
         <v>18</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="N64" s="4" t="s">
         <v>62</v>
       </c>
       <c r="O64" s="4" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="Q64" s="4" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="S64" s="4" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="U64" s="4" t="s">
         <v>36</v>
       </c>
       <c r="V64" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="W64" s="4" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="X64" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="Y64" s="4" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="AA64" s="4" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="AB64" s="4" t="s">
         <v>54</v>
       </c>
       <c r="AC64" s="4" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="AF64" s="5" t="n">
         <v>18</v>
@@ -5292,16 +5352,16 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="4" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>69</v>
@@ -5309,16 +5369,16 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="4" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>69</v>
@@ -5326,16 +5386,16 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="4" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>69</v>
@@ -5343,22 +5403,22 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="4" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="K68" s="5" t="n">
         <v>14</v>
@@ -5369,16 +5429,16 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="4" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>69</v>
@@ -5386,73 +5446,73 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="4" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="4" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>69</v>
       </c>
       <c r="AI71" s="4" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="4" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>69</v>
       </c>
       <c r="AI72" s="4" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="4" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>69</v>
@@ -5460,176 +5520,176 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="4" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>69</v>
       </c>
       <c r="AI74" s="4" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="4" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="4" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="4" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="4" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="4" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="4" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="4" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="G81" s="4" t="s">
         <v>69</v>
       </c>
       <c r="AI81" s="4" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="4" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="I82" s="4" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K82" s="5" t="n">
         <v>17</v>
       </c>
       <c r="L82" s="4" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="AF82" s="5" t="n">
         <v>17</v>
@@ -5637,28 +5697,28 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="4" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="K83" s="5" t="n">
         <v>15</v>
       </c>
       <c r="M83" s="4" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="N83" s="4" t="s">
         <v>62</v>
@@ -5669,28 +5729,28 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="4" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H84" s="4" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="I84" s="4" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="K84" s="5" t="n">
         <v>15</v>
@@ -5701,33 +5761,33 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="4" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G85" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="4" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="G86" s="4" t="s">
         <v>69</v>
@@ -5736,114 +5796,114 @@
         <v>58</v>
       </c>
       <c r="I86" s="4" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="J86" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K86" s="5" t="n">
         <v>17</v>
       </c>
       <c r="L86" s="4" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="M86" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N86" s="4" t="s">
         <v>62</v>
       </c>
       <c r="O86" s="4" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="P86" s="4" t="s">
         <v>46</v>
       </c>
       <c r="Q86" s="4" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="S86" s="4" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="V86" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="W86" s="4" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="X86" s="4" t="s">
         <v>51</v>
       </c>
       <c r="Y86" s="4" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="AA86" s="4" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="AB86" s="4" t="s">
         <v>54</v>
       </c>
       <c r="AC86" s="4" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="AF86" s="5" t="n">
         <v>17</v>
       </c>
       <c r="AI86" s="4" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="4" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H87" s="4" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="K87" s="5" t="n">
         <v>15</v>
       </c>
       <c r="L87" s="4" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="M87" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N87" s="4" t="s">
         <v>62</v>
       </c>
       <c r="O87" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="P87" s="4" t="s">
         <v>46</v>
       </c>
       <c r="Q87" s="4" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="R87" s="4" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="S87" s="4" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="U87" s="4" t="s">
         <v>36</v>
@@ -5855,269 +5915,269 @@
         <v>51</v>
       </c>
       <c r="AB87" s="4" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="AF87" s="5" t="n">
         <v>15</v>
       </c>
       <c r="AI87" s="4" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="4" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="4" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="4" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="4" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="4" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="4" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="4" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="4" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="4" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="4" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="AD97" s="4" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="4" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="4" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="4" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="4" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="4" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="4" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="4" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="4" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="4" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="4" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="4" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="4" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="4" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="E110" s="4" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
     </row>
   </sheetData>

</xml_diff>